<commit_message>
odds ratio and p value calculation function is written
</commit_message>
<xml_diff>
--- a/LOR Project_expanded.xlsx
+++ b/LOR Project_expanded.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\GIT\AURA_REFERENCE_LETTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47979F6-18E2-41F1-A175-374DF4AA851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3AAC3D-1071-4832-B436-EEBB4F775946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographics" sheetId="1" r:id="rId1"/>
@@ -1945,61 +1945,61 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3042,7 +3042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:X62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
@@ -3066,8 +3066,8 @@
     </row>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="94"/>
-      <c r="C4" s="93" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="90" t="s">
         <v>156</v>
       </c>
       <c r="D4" s="78"/>
@@ -3075,15 +3075,15 @@
       <c r="F4" s="78"/>
       <c r="G4" s="78"/>
       <c r="H4" s="80"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="93"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="90"/>
       <c r="L4" s="78"/>
       <c r="M4" s="78"/>
       <c r="N4" s="78"/>
       <c r="O4" s="78"/>
       <c r="P4" s="80"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="93"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="90"/>
       <c r="T4" s="78"/>
       <c r="U4" s="78"/>
       <c r="V4" s="78"/>
@@ -3091,54 +3091,54 @@
       <c r="X4" s="80"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="95"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="99" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="100"/>
-      <c r="E5" s="87" t="s">
+      <c r="E5" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="88"/>
-      <c r="G5" s="97" t="s">
+      <c r="F5" s="102"/>
+      <c r="G5" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="H5" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="J5" s="95"/>
+      <c r="J5" s="88"/>
       <c r="K5" s="99" t="s">
         <v>184</v>
       </c>
       <c r="L5" s="100"/>
-      <c r="M5" s="87" t="s">
+      <c r="M5" s="101" t="s">
         <v>186</v>
       </c>
-      <c r="N5" s="88"/>
-      <c r="O5" s="97" t="s">
+      <c r="N5" s="102"/>
+      <c r="O5" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="P5" s="89" t="s">
+      <c r="P5" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="R5" s="95"/>
+      <c r="R5" s="88"/>
       <c r="S5" s="99" t="s">
         <v>185</v>
       </c>
       <c r="T5" s="100"/>
-      <c r="U5" s="87" t="s">
+      <c r="U5" s="101" t="s">
         <v>187</v>
       </c>
-      <c r="V5" s="88"/>
-      <c r="W5" s="97" t="s">
+      <c r="V5" s="102"/>
+      <c r="W5" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="X5" s="89" t="s">
+      <c r="X5" s="97" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="96"/>
+      <c r="B6" s="89"/>
       <c r="C6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3151,9 +3151,9 @@
       <c r="F6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="90"/>
-      <c r="J6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="98"/>
+      <c r="J6" s="89"/>
       <c r="K6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3166,9 +3166,9 @@
       <c r="N6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="98"/>
-      <c r="P6" s="90"/>
-      <c r="R6" s="96"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="98"/>
+      <c r="R6" s="89"/>
       <c r="S6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3181,8 +3181,8 @@
       <c r="V6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="98"/>
-      <c r="X6" s="90"/>
+      <c r="W6" s="96"/>
+      <c r="X6" s="98"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
@@ -3408,8 +3408,8 @@
     </row>
     <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="94"/>
-      <c r="C14" s="93" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="90" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="78"/>
@@ -3419,19 +3419,19 @@
       <c r="H14" s="80"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="95"/>
+      <c r="B15" s="88"/>
       <c r="C15" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="88"/>
-      <c r="E15" s="87" t="s">
+      <c r="D15" s="102"/>
+      <c r="E15" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="88"/>
-      <c r="G15" s="104" t="s">
+      <c r="F15" s="102"/>
+      <c r="G15" s="103" t="s">
         <v>158</v>
       </c>
-      <c r="H15" s="103" t="s">
+      <c r="H15" s="105" t="s">
         <v>157</v>
       </c>
       <c r="O15" t="s">
@@ -3442,7 +3442,7 @@
       </c>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="96"/>
+      <c r="B16" s="89"/>
       <c r="C16" s="42" t="s">
         <v>7</v>
       </c>
@@ -3455,8 +3455,8 @@
       <c r="F16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="105"/>
-      <c r="H16" s="90"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="98"/>
       <c r="N16" t="s">
         <v>188</v>
       </c>
@@ -3613,8 +3613,8 @@
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="94"/>
-      <c r="C24" s="93" t="s">
+      <c r="B24" s="87"/>
+      <c r="C24" s="90" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="78"/>
@@ -3631,32 +3631,32 @@
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="95"/>
-      <c r="C25" s="101" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="91" t="s">
+      <c r="D25" s="92"/>
+      <c r="E25" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="F25" s="92"/>
-      <c r="G25" s="101" t="s">
+      <c r="F25" s="94"/>
+      <c r="G25" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="102"/>
-      <c r="I25" s="91" t="s">
+      <c r="H25" s="92"/>
+      <c r="I25" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="J25" s="92"/>
-      <c r="K25" s="97" t="s">
+      <c r="J25" s="94"/>
+      <c r="K25" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="L25" s="89" t="s">
+      <c r="L25" s="97" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="96"/>
+      <c r="B26" s="89"/>
       <c r="C26" s="44" t="s">
         <v>7</v>
       </c>
@@ -3681,8 +3681,8 @@
       <c r="J26" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="98"/>
-      <c r="L26" s="90"/>
+      <c r="K26" s="96"/>
+      <c r="L26" s="98"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="32" t="s">
@@ -3871,8 +3871,8 @@
     </row>
     <row r="33" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="94"/>
-      <c r="C34" s="93" t="s">
+      <c r="B34" s="87"/>
+      <c r="C34" s="90" t="s">
         <v>178</v>
       </c>
       <c r="D34" s="78"/>
@@ -3884,8 +3884,8 @@
       <c r="J34" s="78"/>
       <c r="K34" s="78"/>
       <c r="L34" s="80"/>
-      <c r="N34" s="94"/>
-      <c r="O34" s="93" t="s">
+      <c r="N34" s="87"/>
+      <c r="O34" s="90" t="s">
         <v>179</v>
       </c>
       <c r="P34" s="78"/>
@@ -3899,55 +3899,55 @@
       <c r="X34" s="80"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" s="95"/>
-      <c r="C35" s="101" t="s">
+      <c r="B35" s="88"/>
+      <c r="C35" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="102"/>
-      <c r="E35" s="91" t="s">
+      <c r="D35" s="92"/>
+      <c r="E35" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="92"/>
-      <c r="G35" s="101" t="s">
+      <c r="F35" s="94"/>
+      <c r="G35" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="102"/>
-      <c r="I35" s="91" t="s">
+      <c r="H35" s="92"/>
+      <c r="I35" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="J35" s="92"/>
-      <c r="K35" s="97" t="s">
+      <c r="J35" s="94"/>
+      <c r="K35" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="L35" s="89" t="s">
+      <c r="L35" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="N35" s="95"/>
-      <c r="O35" s="101" t="s">
+      <c r="N35" s="88"/>
+      <c r="O35" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="P35" s="102"/>
-      <c r="Q35" s="91" t="s">
+      <c r="P35" s="92"/>
+      <c r="Q35" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="R35" s="92"/>
-      <c r="S35" s="101" t="s">
+      <c r="R35" s="94"/>
+      <c r="S35" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="T35" s="102"/>
-      <c r="U35" s="91" t="s">
+      <c r="T35" s="92"/>
+      <c r="U35" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="V35" s="92"/>
-      <c r="W35" s="97" t="s">
+      <c r="V35" s="94"/>
+      <c r="W35" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="X35" s="89" t="s">
+      <c r="X35" s="97" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="36" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="96"/>
+      <c r="B36" s="89"/>
       <c r="C36" s="44" t="s">
         <v>7</v>
       </c>
@@ -3972,9 +3972,9 @@
       <c r="J36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="98"/>
-      <c r="L36" s="90"/>
-      <c r="N36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="98"/>
+      <c r="N36" s="89"/>
       <c r="O36" s="44" t="s">
         <v>7</v>
       </c>
@@ -3999,8 +3999,8 @@
       <c r="V36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W36" s="98"/>
-      <c r="X36" s="90"/>
+      <c r="W36" s="96"/>
+      <c r="X36" s="98"/>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="32" t="s">
@@ -4170,8 +4170,8 @@
     </row>
     <row r="43" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" s="94"/>
-      <c r="C44" s="93" t="s">
+      <c r="B44" s="87"/>
+      <c r="C44" s="90" t="s">
         <v>180</v>
       </c>
       <c r="D44" s="78"/>
@@ -4183,8 +4183,8 @@
       <c r="J44" s="78"/>
       <c r="K44" s="78"/>
       <c r="L44" s="80"/>
-      <c r="N44" s="94"/>
-      <c r="O44" s="93" t="s">
+      <c r="N44" s="87"/>
+      <c r="O44" s="90" t="s">
         <v>181</v>
       </c>
       <c r="P44" s="78"/>
@@ -4198,55 +4198,55 @@
       <c r="X44" s="80"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="95"/>
-      <c r="C45" s="101" t="s">
+      <c r="B45" s="88"/>
+      <c r="C45" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="102"/>
-      <c r="E45" s="91" t="s">
+      <c r="D45" s="92"/>
+      <c r="E45" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="F45" s="92"/>
-      <c r="G45" s="101" t="s">
+      <c r="F45" s="94"/>
+      <c r="G45" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H45" s="102"/>
-      <c r="I45" s="91" t="s">
+      <c r="H45" s="92"/>
+      <c r="I45" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="J45" s="92"/>
-      <c r="K45" s="97" t="s">
+      <c r="J45" s="94"/>
+      <c r="K45" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="L45" s="89" t="s">
+      <c r="L45" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="N45" s="95"/>
-      <c r="O45" s="101" t="s">
+      <c r="N45" s="88"/>
+      <c r="O45" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="P45" s="102"/>
-      <c r="Q45" s="91" t="s">
+      <c r="P45" s="92"/>
+      <c r="Q45" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="R45" s="92"/>
-      <c r="S45" s="101" t="s">
+      <c r="R45" s="94"/>
+      <c r="S45" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="T45" s="102"/>
-      <c r="U45" s="91" t="s">
+      <c r="T45" s="92"/>
+      <c r="U45" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="V45" s="92"/>
-      <c r="W45" s="97" t="s">
+      <c r="V45" s="94"/>
+      <c r="W45" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="X45" s="89" t="s">
+      <c r="X45" s="97" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="46" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="96"/>
+      <c r="B46" s="89"/>
       <c r="C46" s="44" t="s">
         <v>7</v>
       </c>
@@ -4271,9 +4271,9 @@
       <c r="J46" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="98"/>
-      <c r="L46" s="90"/>
-      <c r="N46" s="96"/>
+      <c r="K46" s="96"/>
+      <c r="L46" s="98"/>
+      <c r="N46" s="89"/>
       <c r="O46" s="44" t="s">
         <v>7</v>
       </c>
@@ -4298,8 +4298,8 @@
       <c r="V46" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W46" s="98"/>
-      <c r="X46" s="90"/>
+      <c r="W46" s="96"/>
+      <c r="X46" s="98"/>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
@@ -4469,8 +4469,8 @@
     </row>
     <row r="53" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B54" s="94"/>
-      <c r="C54" s="93" t="s">
+      <c r="B54" s="87"/>
+      <c r="C54" s="90" t="s">
         <v>182</v>
       </c>
       <c r="D54" s="78"/>
@@ -4482,8 +4482,8 @@
       <c r="J54" s="78"/>
       <c r="K54" s="78"/>
       <c r="L54" s="80"/>
-      <c r="N54" s="94"/>
-      <c r="O54" s="93" t="s">
+      <c r="N54" s="87"/>
+      <c r="O54" s="90" t="s">
         <v>183</v>
       </c>
       <c r="P54" s="78"/>
@@ -4497,55 +4497,55 @@
       <c r="X54" s="80"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B55" s="95"/>
-      <c r="C55" s="101" t="s">
+      <c r="B55" s="88"/>
+      <c r="C55" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="102"/>
-      <c r="E55" s="91" t="s">
+      <c r="D55" s="92"/>
+      <c r="E55" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="F55" s="92"/>
-      <c r="G55" s="101" t="s">
+      <c r="F55" s="94"/>
+      <c r="G55" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="H55" s="102"/>
-      <c r="I55" s="91" t="s">
+      <c r="H55" s="92"/>
+      <c r="I55" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="J55" s="92"/>
-      <c r="K55" s="97" t="s">
+      <c r="J55" s="94"/>
+      <c r="K55" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="L55" s="89" t="s">
+      <c r="L55" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="N55" s="95"/>
-      <c r="O55" s="101" t="s">
+      <c r="N55" s="88"/>
+      <c r="O55" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="P55" s="102"/>
-      <c r="Q55" s="91" t="s">
+      <c r="P55" s="92"/>
+      <c r="Q55" s="93" t="s">
         <v>168</v>
       </c>
-      <c r="R55" s="92"/>
-      <c r="S55" s="101" t="s">
+      <c r="R55" s="94"/>
+      <c r="S55" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="T55" s="102"/>
-      <c r="U55" s="91" t="s">
+      <c r="T55" s="92"/>
+      <c r="U55" s="93" t="s">
         <v>169</v>
       </c>
-      <c r="V55" s="92"/>
-      <c r="W55" s="97" t="s">
+      <c r="V55" s="94"/>
+      <c r="W55" s="95" t="s">
         <v>158</v>
       </c>
-      <c r="X55" s="89" t="s">
+      <c r="X55" s="97" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="56" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="96"/>
+      <c r="B56" s="89"/>
       <c r="C56" s="44" t="s">
         <v>7</v>
       </c>
@@ -4570,9 +4570,9 @@
       <c r="J56" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K56" s="98"/>
-      <c r="L56" s="90"/>
-      <c r="N56" s="96"/>
+      <c r="K56" s="96"/>
+      <c r="L56" s="98"/>
+      <c r="N56" s="89"/>
       <c r="O56" s="44" t="s">
         <v>7</v>
       </c>
@@ -4597,8 +4597,8 @@
       <c r="V56" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W56" s="98"/>
-      <c r="X56" s="90"/>
+      <c r="W56" s="96"/>
+      <c r="X56" s="98"/>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" s="32" t="s">
@@ -4768,6 +4768,70 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="L25:L26"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:X4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="O34:X34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="W35:W36"/>
+    <mergeCell ref="X35:X36"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:L44"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:X44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="W45:W46"/>
+    <mergeCell ref="X45:X46"/>
     <mergeCell ref="B54:B56"/>
     <mergeCell ref="C54:L54"/>
     <mergeCell ref="N54:N56"/>
@@ -4784,70 +4848,6 @@
     <mergeCell ref="U55:V55"/>
     <mergeCell ref="W55:W56"/>
     <mergeCell ref="X55:X56"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:X44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:W46"/>
-    <mergeCell ref="X45:X46"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="O34:X34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="W35:W36"/>
-    <mergeCell ref="X35:X36"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:L34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:X4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="C24:L24"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="K25:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
All word type analysis is done
</commit_message>
<xml_diff>
--- a/LOR Project_expanded.xlsx
+++ b/LOR Project_expanded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\GIT\AURA_REFERENCE_LETTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3AAC3D-1071-4832-B436-EEBB4F775946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3428BDE-B37E-410A-84FC-4E1D45CE3FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -726,7 +726,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -745,8 +745,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="81">
+  <borders count="79">
     <border>
       <left/>
       <right/>
@@ -1675,37 +1681,11 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1777,7 +1757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1882,14 +1862,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="74" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="75" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="76" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="74" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="77" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1899,7 +1874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="78" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="76" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1954,31 +1929,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="78" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="77" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1987,21 +1977,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="63" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="80" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="79" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="75" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="73" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -2456,7 +2434,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q13" sqref="Q13"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,60 +2450,60 @@
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="74"/>
-      <c r="C4" s="72" t="s">
+      <c r="B4" s="69"/>
+      <c r="C4" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="77" t="s">
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="78"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="78" t="s">
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="80"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="75"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="75"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="81" t="s">
+      <c r="B5" s="70"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="84"/>
-      <c r="H5" s="81" t="s">
+      <c r="G5" s="79"/>
+      <c r="H5" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83" t="s">
+      <c r="I5" s="77"/>
+      <c r="J5" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="84"/>
-      <c r="L5" s="85" t="s">
+      <c r="K5" s="79"/>
+      <c r="L5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="83" t="s">
+      <c r="M5" s="77"/>
+      <c r="N5" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="86"/>
+      <c r="O5" s="81"/>
     </row>
     <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="76"/>
-      <c r="C6" s="66" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="62" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="39" t="s">
@@ -2569,8 +2547,8 @@
       <c r="B7" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="C7" s="67">
-        <v>313</v>
+      <c r="C7" s="101">
+        <v>336</v>
       </c>
       <c r="D7" s="60">
         <v>244</v>
@@ -2605,8 +2583,8 @@
       <c r="B8" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="67">
-        <v>964</v>
+      <c r="C8" s="101">
+        <v>1036</v>
       </c>
       <c r="D8" s="33">
         <v>753</v>
@@ -2641,7 +2619,7 @@
       <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="102"/>
       <c r="D9" s="61"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
@@ -2659,19 +2637,19 @@
       <c r="B10" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="C10" s="64">
-        <v>3.0790000000000002</v>
+      <c r="C10" s="102">
+        <v>3.0832999999999999</v>
       </c>
       <c r="D10" s="12">
         <v>3.0859999999999999</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="64" t="s">
         <v>177</v>
       </c>
       <c r="F10" s="11">
         <v>3.0569999999999999</v>
       </c>
-      <c r="G10" s="70" t="s">
+      <c r="G10" s="65" t="s">
         <v>177</v>
       </c>
       <c r="H10" s="12"/>
@@ -2681,13 +2659,13 @@
       <c r="L10" s="12">
         <v>3.133</v>
       </c>
-      <c r="M10" s="69" t="s">
+      <c r="M10" s="64" t="s">
         <v>177</v>
       </c>
       <c r="N10" s="11">
         <v>3.0579999999999998</v>
       </c>
-      <c r="O10" s="68" t="s">
+      <c r="O10" s="63" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2695,19 +2673,19 @@
       <c r="B11" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="C11" s="64">
-        <v>18.420000000000002</v>
+      <c r="C11" s="103">
+        <v>18.388000000000002</v>
       </c>
       <c r="D11" s="12">
         <v>18.309000000000001</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="64" t="s">
         <v>177</v>
       </c>
       <c r="F11" s="11">
         <v>18.818999999999999</v>
       </c>
-      <c r="G11" s="70" t="s">
+      <c r="G11" s="65" t="s">
         <v>177</v>
       </c>
       <c r="H11" s="12"/>
@@ -2717,13 +2695,13 @@
       <c r="L11" s="12">
         <v>18.013999999999999</v>
       </c>
-      <c r="M11" s="69" t="s">
+      <c r="M11" s="64" t="s">
         <v>177</v>
       </c>
       <c r="N11" s="11">
         <v>18.588999999999999</v>
       </c>
-      <c r="O11" s="68" t="s">
+      <c r="O11" s="63" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2731,19 +2709,19 @@
       <c r="B12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="64">
-        <v>346.45299999999997</v>
+      <c r="C12" s="103">
+        <v>344.50799999999998</v>
       </c>
       <c r="D12" s="12">
         <v>346.26</v>
       </c>
-      <c r="E12" s="69" t="s">
+      <c r="E12" s="64" t="s">
         <v>177</v>
       </c>
       <c r="F12" s="11">
         <v>347.142</v>
       </c>
-      <c r="G12" s="70" t="s">
+      <c r="G12" s="65" t="s">
         <v>177</v>
       </c>
       <c r="H12" s="12"/>
@@ -2753,13 +2731,13 @@
       <c r="L12" s="12">
         <v>342.89</v>
       </c>
-      <c r="M12" s="69" t="s">
+      <c r="M12" s="64" t="s">
         <v>177</v>
       </c>
       <c r="N12" s="11">
         <v>347.92599999999999</v>
       </c>
-      <c r="O12" s="68" t="s">
+      <c r="O12" s="63" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2767,7 +2745,7 @@
       <c r="B13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="63"/>
+      <c r="C13" s="102"/>
       <c r="D13" s="18"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
@@ -2785,8 +2763,8 @@
       <c r="B14" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="62">
-        <v>183</v>
+      <c r="C14" s="103">
+        <v>198</v>
       </c>
       <c r="D14" s="12">
         <v>135</v>
@@ -2821,8 +2799,8 @@
       <c r="B15" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="62">
-        <v>767</v>
+      <c r="C15" s="103">
+        <v>824</v>
       </c>
       <c r="D15" s="12">
         <v>610</v>
@@ -2857,7 +2835,7 @@
       <c r="B16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="63"/>
+      <c r="C16" s="102"/>
       <c r="D16" s="18"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
@@ -2875,8 +2853,8 @@
       <c r="B17" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="62">
-        <v>171</v>
+      <c r="C17" s="103">
+        <v>193</v>
       </c>
       <c r="D17" s="14">
         <v>134</v>
@@ -2911,8 +2889,8 @@
       <c r="B18" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="62">
-        <v>155</v>
+      <c r="C18" s="103">
+        <v>174</v>
       </c>
       <c r="D18" s="14">
         <v>120</v>
@@ -2947,8 +2925,8 @@
       <c r="B19" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="64">
-        <v>236</v>
+      <c r="C19" s="103">
+        <v>234</v>
       </c>
       <c r="D19" s="14">
         <v>176</v>
@@ -2983,8 +2961,8 @@
       <c r="B20" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C20" s="65">
-        <v>397</v>
+      <c r="C20" s="103">
+        <v>427</v>
       </c>
       <c r="D20" s="24">
         <v>319</v>
@@ -3042,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:X62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="U21" sqref="U21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3066,79 +3044,79 @@
     </row>
     <row r="3" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="87"/>
-      <c r="C4" s="90" t="s">
+      <c r="B4" s="82"/>
+      <c r="C4" s="95" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="78"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="80"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="78"/>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="80"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="90"/>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="80"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="75"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="75"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="75"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B5" s="88"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="99" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="100"/>
-      <c r="E5" s="101" t="s">
+      <c r="E5" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="102"/>
-      <c r="G5" s="95" t="s">
+      <c r="F5" s="92"/>
+      <c r="G5" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="J5" s="88"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="99" t="s">
         <v>184</v>
       </c>
       <c r="L5" s="100"/>
-      <c r="M5" s="101" t="s">
+      <c r="M5" s="91" t="s">
         <v>186</v>
       </c>
-      <c r="N5" s="102"/>
-      <c r="O5" s="95" t="s">
+      <c r="N5" s="92"/>
+      <c r="O5" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="P5" s="97" t="s">
+      <c r="P5" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="R5" s="88"/>
+      <c r="R5" s="83"/>
       <c r="S5" s="99" t="s">
         <v>185</v>
       </c>
       <c r="T5" s="100"/>
-      <c r="U5" s="101" t="s">
+      <c r="U5" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="V5" s="102"/>
-      <c r="W5" s="95" t="s">
+      <c r="V5" s="92"/>
+      <c r="W5" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="X5" s="97" t="s">
+      <c r="X5" s="93" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="89"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3151,9 +3129,9 @@
       <c r="F6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="98"/>
-      <c r="J6" s="89"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="94"/>
+      <c r="J6" s="84"/>
       <c r="K6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3166,9 +3144,9 @@
       <c r="N6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="96"/>
-      <c r="P6" s="98"/>
-      <c r="R6" s="89"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="94"/>
+      <c r="R6" s="84"/>
       <c r="S6" s="42" t="s">
         <v>7</v>
       </c>
@@ -3181,27 +3159,31 @@
       <c r="V6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="W6" s="96"/>
-      <c r="X6" s="98"/>
+      <c r="W6" s="86"/>
+      <c r="X6" s="94"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="33">
-        <v>943</v>
-      </c>
-      <c r="D7" s="46">
-        <v>1.2869999999999999</v>
-      </c>
-      <c r="E7" s="37">
-        <v>3138</v>
-      </c>
-      <c r="F7" s="38">
-        <v>1.2030000000000001</v>
-      </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="35"/>
+      <c r="C7">
+        <v>923</v>
+      </c>
+      <c r="D7">
+        <v>43.785578747628001</v>
+      </c>
+      <c r="E7">
+        <v>3626</v>
+      </c>
+      <c r="F7">
+        <v>44.117289207932799</v>
+      </c>
+      <c r="G7">
+        <v>0.99409937888198696</v>
+      </c>
+      <c r="H7">
+        <v>0.90709040817363595</v>
+      </c>
       <c r="J7" s="32" t="s">
         <v>159</v>
       </c>
@@ -3214,8 +3196,6 @@
       <c r="R7" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="S7" s="33"/>
-      <c r="T7" s="46"/>
       <c r="U7" s="37"/>
       <c r="V7" s="38"/>
       <c r="W7" s="33"/>
@@ -3225,20 +3205,24 @@
       <c r="B8" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="14">
-        <v>205</v>
-      </c>
-      <c r="D8" s="47">
-        <v>0.27900000000000003</v>
-      </c>
-      <c r="E8" s="12">
-        <v>645</v>
-      </c>
-      <c r="F8" s="13">
-        <v>0.247</v>
-      </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="20"/>
+      <c r="C8">
+        <v>447</v>
+      </c>
+      <c r="D8">
+        <v>21.204933586337699</v>
+      </c>
+      <c r="E8">
+        <v>1524</v>
+      </c>
+      <c r="F8">
+        <v>18.5424017520379</v>
+      </c>
+      <c r="G8">
+        <v>0.94432034270465603</v>
+      </c>
+      <c r="H8">
+        <v>0.34589726275741001</v>
+      </c>
       <c r="J8" s="30" t="s">
         <v>160</v>
       </c>
@@ -3251,8 +3235,6 @@
       <c r="R8" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="S8" s="14"/>
-      <c r="T8" s="47"/>
       <c r="U8" s="12"/>
       <c r="V8" s="13"/>
       <c r="W8" s="14"/>
@@ -3262,20 +3244,24 @@
       <c r="B9" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="14">
-        <v>164</v>
-      </c>
-      <c r="D9" s="47">
-        <v>0.223</v>
-      </c>
-      <c r="E9" s="12">
-        <v>644</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0.246</v>
-      </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="20"/>
+      <c r="C9">
+        <v>255</v>
+      </c>
+      <c r="D9">
+        <v>12.096774193548301</v>
+      </c>
+      <c r="E9">
+        <v>910</v>
+      </c>
+      <c r="F9">
+        <v>11.071906557975399</v>
+      </c>
+      <c r="G9">
+        <v>0.87773265350388296</v>
+      </c>
+      <c r="H9">
+        <v>8.4843098741095094E-2</v>
+      </c>
       <c r="J9" s="30" t="s">
         <v>114</v>
       </c>
@@ -3288,8 +3274,6 @@
       <c r="R9" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="S9" s="14"/>
-      <c r="T9" s="47"/>
       <c r="U9" s="12"/>
       <c r="V9" s="13"/>
       <c r="W9" s="14"/>
@@ -3299,20 +3283,24 @@
       <c r="B10" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C10" s="14">
-        <v>248</v>
-      </c>
-      <c r="D10" s="47">
-        <v>0.33800000000000002</v>
-      </c>
-      <c r="E10" s="12">
-        <v>944</v>
-      </c>
-      <c r="F10" s="13">
-        <v>362</v>
-      </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="20"/>
+      <c r="C10">
+        <v>407</v>
+      </c>
+      <c r="D10">
+        <v>19.3074003795066</v>
+      </c>
+      <c r="E10">
+        <v>1888</v>
+      </c>
+      <c r="F10">
+        <v>22.971164375228099</v>
+      </c>
+      <c r="G10">
+        <v>1.08364426365905</v>
+      </c>
+      <c r="H10">
+        <v>0.147364966597576</v>
+      </c>
       <c r="J10" s="30" t="s">
         <v>132</v>
       </c>
@@ -3325,8 +3313,6 @@
       <c r="R10" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="S10" s="14"/>
-      <c r="T10" s="47"/>
       <c r="U10" s="12"/>
       <c r="V10" s="13"/>
       <c r="W10" s="14"/>
@@ -3336,20 +3322,24 @@
       <c r="B11" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C11" s="53">
-        <v>17</v>
-      </c>
-      <c r="D11" s="54">
-        <v>2.3E-2</v>
-      </c>
-      <c r="E11" s="55">
-        <v>55</v>
-      </c>
-      <c r="F11" s="56">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="57"/>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>1.1385199240986701</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>1.2166930283489401</v>
+      </c>
+      <c r="G11">
+        <v>1.1609541610079399</v>
+      </c>
+      <c r="H11">
+        <v>0.45969255214655602</v>
+      </c>
       <c r="J11" s="52" t="s">
         <v>153</v>
       </c>
@@ -3362,8 +3352,6 @@
       <c r="R11" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="S11" s="53"/>
-      <c r="T11" s="54"/>
       <c r="U11" s="55"/>
       <c r="V11" s="56"/>
       <c r="W11" s="53"/>
@@ -3373,20 +3361,24 @@
       <c r="B12" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="24">
-        <v>54</v>
-      </c>
-      <c r="D12" s="48">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="E12" s="21">
-        <v>149</v>
-      </c>
-      <c r="F12" s="23">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
+      <c r="C12">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>2.4667931688804501</v>
+      </c>
+      <c r="E12">
+        <v>171</v>
+      </c>
+      <c r="F12">
+        <v>2.0805450784767001</v>
+      </c>
+      <c r="G12">
+        <v>1.3567519019442</v>
+      </c>
+      <c r="H12">
+        <v>4.6778222756434999E-2</v>
+      </c>
       <c r="J12" s="31" t="s">
         <v>154</v>
       </c>
@@ -3399,8 +3391,6 @@
       <c r="R12" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="S12" s="24"/>
-      <c r="T12" s="48"/>
       <c r="U12" s="21"/>
       <c r="V12" s="23"/>
       <c r="W12" s="24"/>
@@ -3408,30 +3398,30 @@
     </row>
     <row r="13" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="87"/>
-      <c r="C14" s="90" t="s">
+      <c r="B14" s="82"/>
+      <c r="C14" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
-      <c r="H14" s="80"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="75"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="88"/>
+      <c r="B15" s="83"/>
       <c r="C15" s="99" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="102"/>
-      <c r="E15" s="101" t="s">
+      <c r="D15" s="92"/>
+      <c r="E15" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103" t="s">
+      <c r="F15" s="92"/>
+      <c r="G15" s="96" t="s">
         <v>158</v>
       </c>
-      <c r="H15" s="105" t="s">
+      <c r="H15" s="98" t="s">
         <v>157</v>
       </c>
       <c r="O15" t="s">
@@ -3442,7 +3432,7 @@
       </c>
     </row>
     <row r="16" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="89"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="42" t="s">
         <v>7</v>
       </c>
@@ -3455,8 +3445,8 @@
       <c r="F16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="104"/>
-      <c r="H16" s="98"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="94"/>
       <c r="N16" t="s">
         <v>188</v>
       </c>
@@ -3471,18 +3461,8 @@
       <c r="B17" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C17" s="33">
-        <v>828</v>
-      </c>
-      <c r="D17" s="34">
-        <v>1.21</v>
-      </c>
-      <c r="E17" s="34">
-        <v>3215</v>
-      </c>
-      <c r="F17" s="34">
-        <v>1.2290000000000001</v>
-      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
       <c r="G17" s="34"/>
       <c r="H17" s="35"/>
       <c r="N17" t="s">
@@ -3499,18 +3479,8 @@
       <c r="B18" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C18" s="14">
-        <v>188</v>
-      </c>
-      <c r="D18" s="11">
-        <v>0.27400000000000002</v>
-      </c>
-      <c r="E18" s="11">
-        <v>645</v>
-      </c>
-      <c r="F18" s="11">
-        <v>0.246</v>
-      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="11"/>
       <c r="G18" s="11"/>
       <c r="H18" s="20"/>
     </row>
@@ -3518,18 +3488,8 @@
       <c r="B19" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="14">
-        <v>180</v>
-      </c>
-      <c r="D19" s="11">
-        <v>0.26300000000000001</v>
-      </c>
-      <c r="E19" s="11">
-        <v>619</v>
-      </c>
-      <c r="F19" s="11">
-        <v>0.23599999999999999</v>
-      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="20"/>
       <c r="N19" t="s">
@@ -3540,18 +3500,8 @@
       <c r="B20" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="14">
-        <v>217</v>
-      </c>
-      <c r="D20" s="11">
-        <v>0.317</v>
-      </c>
-      <c r="E20" s="11">
-        <v>966</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0.36899999999999999</v>
-      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="11"/>
       <c r="G20" s="11"/>
       <c r="H20" s="20"/>
       <c r="N20" t="s">
@@ -3565,18 +3515,8 @@
       <c r="B21" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="53">
-        <v>15</v>
-      </c>
-      <c r="D21" s="58">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E21" s="58">
-        <v>57</v>
-      </c>
-      <c r="F21" s="59">
-        <v>2.1000000000000001E-2</v>
-      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="58"/>
       <c r="G21" s="58"/>
       <c r="H21" s="57"/>
       <c r="N21" t="s">
@@ -3590,18 +3530,8 @@
       <c r="B22" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="24">
-        <v>46</v>
-      </c>
-      <c r="D22" s="22">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="E22" s="22">
-        <v>153</v>
-      </c>
-      <c r="F22" s="22">
-        <v>5.8000000000000003E-2</v>
-      </c>
+      <c r="C22" s="24"/>
+      <c r="D22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="25"/>
       <c r="N22" t="s">
@@ -3613,50 +3543,50 @@
     </row>
     <row r="23" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="87"/>
-      <c r="C24" s="90" t="s">
+      <c r="B24" s="82"/>
+      <c r="C24" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="80"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="75"/>
       <c r="N24" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="88"/>
-      <c r="C25" s="91" t="s">
+      <c r="B25" s="83"/>
+      <c r="C25" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D25" s="92"/>
-      <c r="E25" s="93" t="s">
+      <c r="D25" s="88"/>
+      <c r="E25" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="F25" s="94"/>
-      <c r="G25" s="91" t="s">
+      <c r="F25" s="90"/>
+      <c r="G25" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="92"/>
-      <c r="I25" s="93" t="s">
+      <c r="H25" s="88"/>
+      <c r="I25" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="J25" s="94"/>
-      <c r="K25" s="95" t="s">
+      <c r="J25" s="90"/>
+      <c r="K25" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="L25" s="97" t="s">
+      <c r="L25" s="93" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="26" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="89"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="44" t="s">
         <v>7</v>
       </c>
@@ -3681,37 +3611,21 @@
       <c r="J26" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="96"/>
-      <c r="L26" s="98"/>
+      <c r="K26" s="86"/>
+      <c r="L26" s="94"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C27" s="33">
-        <v>715</v>
-      </c>
-      <c r="D27" s="46">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="E27" s="37">
-        <v>756</v>
-      </c>
-      <c r="F27" s="38">
-        <v>1.266</v>
-      </c>
-      <c r="G27" s="33">
-        <v>999</v>
-      </c>
-      <c r="H27" s="46">
-        <v>1.252</v>
-      </c>
-      <c r="I27" s="37">
-        <v>1593</v>
-      </c>
-      <c r="J27" s="38">
-        <v>1.2130000000000001</v>
-      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
       <c r="K27" s="33"/>
       <c r="L27" s="35"/>
     </row>
@@ -3719,30 +3633,14 @@
       <c r="B28" s="30" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="14">
-        <v>154</v>
-      </c>
-      <c r="D28" s="47">
-        <v>0.25</v>
-      </c>
-      <c r="E28" s="12">
-        <v>159</v>
-      </c>
-      <c r="F28" s="13">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="G28" s="14">
-        <v>184</v>
-      </c>
-      <c r="H28" s="59">
-        <v>0.23</v>
-      </c>
-      <c r="I28" s="12">
-        <v>348</v>
-      </c>
-      <c r="J28" s="13">
-        <v>0.26400000000000001</v>
-      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="14"/>
       <c r="L28" s="20"/>
     </row>
@@ -3750,30 +3648,14 @@
       <c r="B29" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="14">
-        <v>132</v>
-      </c>
-      <c r="D29" s="47">
-        <v>0.214</v>
-      </c>
-      <c r="E29" s="12">
-        <v>152</v>
-      </c>
-      <c r="F29" s="13">
-        <v>0.254</v>
-      </c>
-      <c r="G29" s="14">
-        <v>196</v>
-      </c>
-      <c r="H29" s="47">
-        <v>0.245</v>
-      </c>
-      <c r="I29" s="12">
-        <v>327</v>
-      </c>
-      <c r="J29" s="13">
-        <v>0.249</v>
-      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="14"/>
       <c r="L29" s="20"/>
     </row>
@@ -3781,30 +3663,14 @@
       <c r="B30" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="C30" s="14">
-        <v>275</v>
-      </c>
-      <c r="D30" s="47">
-        <v>0.44600000000000001</v>
-      </c>
-      <c r="E30" s="12">
-        <v>216</v>
-      </c>
-      <c r="F30" s="13">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="G30" s="14">
-        <v>256</v>
-      </c>
-      <c r="H30" s="59">
-        <v>0.32</v>
-      </c>
-      <c r="I30" s="12">
-        <v>442</v>
-      </c>
-      <c r="J30" s="13">
-        <v>0.33600000000000002</v>
-      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="14"/>
       <c r="L30" s="20"/>
     </row>
@@ -3812,142 +3678,110 @@
       <c r="B31" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="C31" s="53">
-        <v>13</v>
-      </c>
-      <c r="D31" s="54">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="E31" s="55">
-        <v>12</v>
-      </c>
-      <c r="F31" s="56">
-        <v>0.02</v>
-      </c>
-      <c r="G31" s="53">
-        <v>15</v>
-      </c>
-      <c r="H31" s="54">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="I31" s="71">
-        <v>32</v>
-      </c>
-      <c r="J31" s="56">
-        <v>2.4E-2</v>
-      </c>
+      <c r="C31" s="53"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="56"/>
       <c r="L31" s="57"/>
     </row>
     <row r="32" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="C32" s="24">
-        <v>39</v>
-      </c>
-      <c r="D32" s="48">
-        <v>6.3E-2</v>
-      </c>
-      <c r="E32" s="21">
-        <v>40</v>
-      </c>
-      <c r="F32" s="23">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="G32" s="23">
-        <v>44</v>
-      </c>
-      <c r="H32" s="23">
-        <v>5.5E-2</v>
-      </c>
-      <c r="I32" s="23">
-        <v>79</v>
-      </c>
-      <c r="J32" s="23">
-        <v>0.06</v>
-      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
       <c r="K32" s="22"/>
       <c r="L32" s="25"/>
     </row>
     <row r="33" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B34" s="87"/>
-      <c r="C34" s="90" t="s">
+      <c r="B34" s="82"/>
+      <c r="C34" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="D34" s="78"/>
-      <c r="E34" s="78"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="78"/>
-      <c r="J34" s="78"/>
-      <c r="K34" s="78"/>
-      <c r="L34" s="80"/>
-      <c r="N34" s="87"/>
-      <c r="O34" s="90" t="s">
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="73"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="75"/>
+      <c r="N34" s="82"/>
+      <c r="O34" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="P34" s="78"/>
-      <c r="Q34" s="78"/>
-      <c r="R34" s="78"/>
-      <c r="S34" s="78"/>
-      <c r="T34" s="78"/>
-      <c r="U34" s="78"/>
-      <c r="V34" s="78"/>
-      <c r="W34" s="78"/>
-      <c r="X34" s="80"/>
+      <c r="P34" s="73"/>
+      <c r="Q34" s="73"/>
+      <c r="R34" s="73"/>
+      <c r="S34" s="73"/>
+      <c r="T34" s="73"/>
+      <c r="U34" s="73"/>
+      <c r="V34" s="73"/>
+      <c r="W34" s="73"/>
+      <c r="X34" s="75"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B35" s="88"/>
-      <c r="C35" s="91" t="s">
+      <c r="B35" s="83"/>
+      <c r="C35" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="92"/>
-      <c r="E35" s="93" t="s">
+      <c r="D35" s="88"/>
+      <c r="E35" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="F35" s="94"/>
-      <c r="G35" s="91" t="s">
+      <c r="F35" s="90"/>
+      <c r="G35" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="H35" s="92"/>
-      <c r="I35" s="93" t="s">
+      <c r="H35" s="88"/>
+      <c r="I35" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="J35" s="94"/>
-      <c r="K35" s="95" t="s">
+      <c r="J35" s="90"/>
+      <c r="K35" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="L35" s="97" t="s">
+      <c r="L35" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="N35" s="88"/>
-      <c r="O35" s="91" t="s">
+      <c r="N35" s="83"/>
+      <c r="O35" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="P35" s="92"/>
-      <c r="Q35" s="93" t="s">
+      <c r="P35" s="88"/>
+      <c r="Q35" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="R35" s="94"/>
-      <c r="S35" s="91" t="s">
+      <c r="R35" s="90"/>
+      <c r="S35" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="T35" s="92"/>
-      <c r="U35" s="93" t="s">
+      <c r="T35" s="88"/>
+      <c r="U35" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="V35" s="94"/>
-      <c r="W35" s="95" t="s">
+      <c r="V35" s="90"/>
+      <c r="W35" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="X35" s="97" t="s">
+      <c r="X35" s="93" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="36" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="89"/>
+      <c r="B36" s="84"/>
       <c r="C36" s="44" t="s">
         <v>7</v>
       </c>
@@ -3972,9 +3806,9 @@
       <c r="J36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K36" s="96"/>
-      <c r="L36" s="98"/>
-      <c r="N36" s="89"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="94"/>
+      <c r="N36" s="84"/>
       <c r="O36" s="44" t="s">
         <v>7</v>
       </c>
@@ -3999,8 +3833,8 @@
       <c r="V36" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W36" s="96"/>
-      <c r="X36" s="98"/>
+      <c r="W36" s="86"/>
+      <c r="X36" s="94"/>
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="32" t="s">
@@ -4124,7 +3958,7 @@
       <c r="F41" s="56"/>
       <c r="G41" s="53"/>
       <c r="H41" s="54"/>
-      <c r="I41" s="71"/>
+      <c r="I41" s="66"/>
       <c r="J41" s="56"/>
       <c r="L41" s="57"/>
       <c r="N41" s="52" t="s">
@@ -4136,7 +3970,7 @@
       <c r="R41" s="56"/>
       <c r="S41" s="53"/>
       <c r="T41" s="54"/>
-      <c r="U41" s="71"/>
+      <c r="U41" s="66"/>
       <c r="V41" s="56"/>
       <c r="X41" s="57"/>
     </row>
@@ -4170,83 +4004,83 @@
     </row>
     <row r="43" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="44" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B44" s="87"/>
-      <c r="C44" s="90" t="s">
+      <c r="B44" s="82"/>
+      <c r="C44" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="D44" s="78"/>
-      <c r="E44" s="78"/>
-      <c r="F44" s="78"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="80"/>
-      <c r="N44" s="87"/>
-      <c r="O44" s="90" t="s">
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="75"/>
+      <c r="N44" s="82"/>
+      <c r="O44" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="P44" s="78"/>
-      <c r="Q44" s="78"/>
-      <c r="R44" s="78"/>
-      <c r="S44" s="78"/>
-      <c r="T44" s="78"/>
-      <c r="U44" s="78"/>
-      <c r="V44" s="78"/>
-      <c r="W44" s="78"/>
-      <c r="X44" s="80"/>
+      <c r="P44" s="73"/>
+      <c r="Q44" s="73"/>
+      <c r="R44" s="73"/>
+      <c r="S44" s="73"/>
+      <c r="T44" s="73"/>
+      <c r="U44" s="73"/>
+      <c r="V44" s="73"/>
+      <c r="W44" s="73"/>
+      <c r="X44" s="75"/>
     </row>
     <row r="45" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B45" s="88"/>
-      <c r="C45" s="91" t="s">
+      <c r="B45" s="83"/>
+      <c r="C45" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="92"/>
-      <c r="E45" s="93" t="s">
+      <c r="D45" s="88"/>
+      <c r="E45" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="F45" s="94"/>
-      <c r="G45" s="91" t="s">
+      <c r="F45" s="90"/>
+      <c r="G45" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="H45" s="92"/>
-      <c r="I45" s="93" t="s">
+      <c r="H45" s="88"/>
+      <c r="I45" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="J45" s="94"/>
-      <c r="K45" s="95" t="s">
+      <c r="J45" s="90"/>
+      <c r="K45" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="L45" s="97" t="s">
+      <c r="L45" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="N45" s="88"/>
-      <c r="O45" s="91" t="s">
+      <c r="N45" s="83"/>
+      <c r="O45" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="P45" s="92"/>
-      <c r="Q45" s="93" t="s">
+      <c r="P45" s="88"/>
+      <c r="Q45" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="R45" s="94"/>
-      <c r="S45" s="91" t="s">
+      <c r="R45" s="90"/>
+      <c r="S45" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="T45" s="92"/>
-      <c r="U45" s="93" t="s">
+      <c r="T45" s="88"/>
+      <c r="U45" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="V45" s="94"/>
-      <c r="W45" s="95" t="s">
+      <c r="V45" s="90"/>
+      <c r="W45" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="X45" s="97" t="s">
+      <c r="X45" s="93" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="46" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="89"/>
+      <c r="B46" s="84"/>
       <c r="C46" s="44" t="s">
         <v>7</v>
       </c>
@@ -4271,9 +4105,9 @@
       <c r="J46" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K46" s="96"/>
-      <c r="L46" s="98"/>
-      <c r="N46" s="89"/>
+      <c r="K46" s="86"/>
+      <c r="L46" s="94"/>
+      <c r="N46" s="84"/>
       <c r="O46" s="44" t="s">
         <v>7</v>
       </c>
@@ -4298,8 +4132,8 @@
       <c r="V46" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W46" s="96"/>
-      <c r="X46" s="98"/>
+      <c r="W46" s="86"/>
+      <c r="X46" s="94"/>
     </row>
     <row r="47" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B47" s="32" t="s">
@@ -4423,7 +4257,7 @@
       <c r="F51" s="56"/>
       <c r="G51" s="53"/>
       <c r="H51" s="54"/>
-      <c r="I51" s="71"/>
+      <c r="I51" s="66"/>
       <c r="J51" s="56"/>
       <c r="L51" s="57"/>
       <c r="N51" s="52" t="s">
@@ -4435,7 +4269,7 @@
       <c r="R51" s="56"/>
       <c r="S51" s="53"/>
       <c r="T51" s="54"/>
-      <c r="U51" s="71"/>
+      <c r="U51" s="66"/>
       <c r="V51" s="56"/>
       <c r="X51" s="57"/>
     </row>
@@ -4469,83 +4303,83 @@
     </row>
     <row r="53" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B54" s="87"/>
-      <c r="C54" s="90" t="s">
+      <c r="B54" s="82"/>
+      <c r="C54" s="95" t="s">
         <v>182</v>
       </c>
-      <c r="D54" s="78"/>
-      <c r="E54" s="78"/>
-      <c r="F54" s="78"/>
-      <c r="G54" s="78"/>
-      <c r="H54" s="78"/>
-      <c r="I54" s="78"/>
-      <c r="J54" s="78"/>
-      <c r="K54" s="78"/>
-      <c r="L54" s="80"/>
-      <c r="N54" s="87"/>
-      <c r="O54" s="90" t="s">
+      <c r="D54" s="73"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="73"/>
+      <c r="I54" s="73"/>
+      <c r="J54" s="73"/>
+      <c r="K54" s="73"/>
+      <c r="L54" s="75"/>
+      <c r="N54" s="82"/>
+      <c r="O54" s="95" t="s">
         <v>183</v>
       </c>
-      <c r="P54" s="78"/>
-      <c r="Q54" s="78"/>
-      <c r="R54" s="78"/>
-      <c r="S54" s="78"/>
-      <c r="T54" s="78"/>
-      <c r="U54" s="78"/>
-      <c r="V54" s="78"/>
-      <c r="W54" s="78"/>
-      <c r="X54" s="80"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
+      <c r="R54" s="73"/>
+      <c r="S54" s="73"/>
+      <c r="T54" s="73"/>
+      <c r="U54" s="73"/>
+      <c r="V54" s="73"/>
+      <c r="W54" s="73"/>
+      <c r="X54" s="75"/>
     </row>
     <row r="55" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B55" s="88"/>
-      <c r="C55" s="91" t="s">
+      <c r="B55" s="83"/>
+      <c r="C55" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="92"/>
-      <c r="E55" s="93" t="s">
+      <c r="D55" s="88"/>
+      <c r="E55" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="F55" s="94"/>
-      <c r="G55" s="91" t="s">
+      <c r="F55" s="90"/>
+      <c r="G55" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="H55" s="92"/>
-      <c r="I55" s="93" t="s">
+      <c r="H55" s="88"/>
+      <c r="I55" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="J55" s="94"/>
-      <c r="K55" s="95" t="s">
+      <c r="J55" s="90"/>
+      <c r="K55" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="L55" s="97" t="s">
+      <c r="L55" s="93" t="s">
         <v>157</v>
       </c>
-      <c r="N55" s="88"/>
-      <c r="O55" s="91" t="s">
+      <c r="N55" s="83"/>
+      <c r="O55" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="P55" s="92"/>
-      <c r="Q55" s="93" t="s">
+      <c r="P55" s="88"/>
+      <c r="Q55" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="R55" s="94"/>
-      <c r="S55" s="91" t="s">
+      <c r="R55" s="90"/>
+      <c r="S55" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="T55" s="92"/>
-      <c r="U55" s="93" t="s">
+      <c r="T55" s="88"/>
+      <c r="U55" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="V55" s="94"/>
-      <c r="W55" s="95" t="s">
+      <c r="V55" s="90"/>
+      <c r="W55" s="85" t="s">
         <v>158</v>
       </c>
-      <c r="X55" s="97" t="s">
+      <c r="X55" s="93" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="56" spans="2:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="89"/>
+      <c r="B56" s="84"/>
       <c r="C56" s="44" t="s">
         <v>7</v>
       </c>
@@ -4570,9 +4404,9 @@
       <c r="J56" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K56" s="96"/>
-      <c r="L56" s="98"/>
-      <c r="N56" s="89"/>
+      <c r="K56" s="86"/>
+      <c r="L56" s="94"/>
+      <c r="N56" s="84"/>
       <c r="O56" s="44" t="s">
         <v>7</v>
       </c>
@@ -4597,8 +4431,8 @@
       <c r="V56" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="W56" s="96"/>
-      <c r="X56" s="98"/>
+      <c r="W56" s="86"/>
+      <c r="X56" s="94"/>
     </row>
     <row r="57" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B57" s="32" t="s">
@@ -4722,7 +4556,7 @@
       <c r="F61" s="56"/>
       <c r="G61" s="53"/>
       <c r="H61" s="54"/>
-      <c r="I61" s="71"/>
+      <c r="I61" s="66"/>
       <c r="J61" s="56"/>
       <c r="L61" s="57"/>
       <c r="N61" s="52" t="s">
@@ -4734,7 +4568,7 @@
       <c r="R61" s="56"/>
       <c r="S61" s="53"/>
       <c r="T61" s="54"/>
-      <c r="U61" s="71"/>
+      <c r="U61" s="66"/>
       <c r="V61" s="56"/>
       <c r="X61" s="57"/>
     </row>
@@ -4768,11 +4602,65 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="N54:N56"/>
+    <mergeCell ref="O54:X54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="K55:K56"/>
+    <mergeCell ref="L55:L56"/>
+    <mergeCell ref="O55:P55"/>
+    <mergeCell ref="Q55:R55"/>
+    <mergeCell ref="S55:T55"/>
+    <mergeCell ref="U55:V55"/>
+    <mergeCell ref="W55:W56"/>
+    <mergeCell ref="X55:X56"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="C44:L44"/>
+    <mergeCell ref="N44:N46"/>
+    <mergeCell ref="O44:X44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="S45:T45"/>
+    <mergeCell ref="U45:V45"/>
+    <mergeCell ref="W45:W46"/>
+    <mergeCell ref="X45:X46"/>
+    <mergeCell ref="N34:N36"/>
+    <mergeCell ref="O34:X34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="S35:T35"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="W35:W36"/>
+    <mergeCell ref="X35:X36"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C34:L34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="L35:L36"/>
+    <mergeCell ref="R4:R6"/>
+    <mergeCell ref="S4:X4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="X5:X6"/>
+    <mergeCell ref="K4:P4"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="L25:L26"/>
     <mergeCell ref="I25:J25"/>
@@ -4789,68 +4677,15 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:P4"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="R4:R6"/>
-    <mergeCell ref="S4:X4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="X5:X6"/>
-    <mergeCell ref="B34:B36"/>
-    <mergeCell ref="C34:L34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K35:K36"/>
-    <mergeCell ref="L35:L36"/>
-    <mergeCell ref="N34:N36"/>
-    <mergeCell ref="O34:X34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="S35:T35"/>
-    <mergeCell ref="U35:V35"/>
-    <mergeCell ref="W35:W36"/>
-    <mergeCell ref="X35:X36"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="N44:N46"/>
-    <mergeCell ref="O44:X44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="S45:T45"/>
-    <mergeCell ref="U45:V45"/>
-    <mergeCell ref="W45:W46"/>
-    <mergeCell ref="X45:X46"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="N54:N56"/>
-    <mergeCell ref="O54:X54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="K55:K56"/>
-    <mergeCell ref="L55:L56"/>
-    <mergeCell ref="O55:P55"/>
-    <mergeCell ref="Q55:R55"/>
-    <mergeCell ref="S55:T55"/>
-    <mergeCell ref="U55:V55"/>
-    <mergeCell ref="W55:W56"/>
-    <mergeCell ref="X55:X56"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" copies="2" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4862,7 +4697,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4870,7 +4705,7 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>